<commit_message>
Update documentation for using Excel and CSV deployments - fix example
</commit_message>
<xml_diff>
--- a/examples/excel/kvm_vsc_upgrade.xlsx
+++ b/examples/excel/kvm_vsc_upgrade.xlsx
@@ -10434,17 +10434,17 @@
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>vcenter</t>
+          <t>kvm</t>
         </is>
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
-          <t>vcenter</t>
+          <t>kvm</t>
         </is>
       </c>
       <c r="D13" s="5" t="inlineStr">
         <is>
-          <t>vcenter</t>
+          <t>kvm</t>
         </is>
       </c>
       <c r="E13" s="5" t="n"/>
@@ -10489,21 +10489,9 @@
           <t>vCenter Datacenter Name</t>
         </is>
       </c>
-      <c r="B16" s="9" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
-      <c r="C16" s="9" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
-      <c r="D16" s="9" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
+      <c r="B16" s="9" t="n"/>
+      <c r="C16" s="9" t="n"/>
+      <c r="D16" s="9" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
       <c r="G16" s="9" t="n"/>
@@ -10514,21 +10502,9 @@
           <t>vCenter Cluster Name</t>
         </is>
       </c>
-      <c r="B17" s="9" t="inlineStr">
-        <is>
-          <t>Cluster-A</t>
-        </is>
-      </c>
-      <c r="C17" s="9" t="inlineStr">
-        <is>
-          <t>Cluster-A</t>
-        </is>
-      </c>
-      <c r="D17" s="9" t="inlineStr">
-        <is>
-          <t>Cluster-B</t>
-        </is>
-      </c>
+      <c r="B17" s="9" t="n"/>
+      <c r="C17" s="9" t="n"/>
+      <c r="D17" s="9" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
       <c r="G17" s="9" t="n"/>
@@ -10552,21 +10528,9 @@
           <t>vCenter Datastore Name</t>
         </is>
       </c>
-      <c r="B19" s="9" t="inlineStr">
-        <is>
-          <t>datastoreA</t>
-        </is>
-      </c>
-      <c r="C19" s="9" t="inlineStr">
-        <is>
-          <t>datastoreA</t>
-        </is>
-      </c>
-      <c r="D19" s="9" t="inlineStr">
-        <is>
-          <t>datastoreB</t>
-        </is>
-      </c>
+      <c r="B19" s="9" t="n"/>
+      <c r="C19" s="9" t="n"/>
+      <c r="D19" s="9" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
       <c r="G19" s="9" t="n"/>
@@ -11340,12 +11304,12 @@
       </c>
       <c r="B23" s="5" t="inlineStr">
         <is>
-          <t>vcenter</t>
+          <t>kvm</t>
         </is>
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>vcenter</t>
+          <t>kvm</t>
         </is>
       </c>
     </row>
@@ -11449,16 +11413,8 @@
           <t>vCenter Datacenter Name</t>
         </is>
       </c>
-      <c r="B34" s="9" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
-      <c r="C34" s="9" t="inlineStr">
-        <is>
-          <t>DC</t>
-        </is>
-      </c>
+      <c r="B34" s="9" t="n"/>
+      <c r="C34" s="9" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="8" t="inlineStr">
@@ -11466,16 +11422,8 @@
           <t>vCenter Cluster Name</t>
         </is>
       </c>
-      <c r="B35" s="9" t="inlineStr">
-        <is>
-          <t>Cluster-A</t>
-        </is>
-      </c>
-      <c r="C35" s="9" t="inlineStr">
-        <is>
-          <t>Cluster-B</t>
-        </is>
-      </c>
+      <c r="B35" s="9" t="n"/>
+      <c r="C35" s="9" t="n"/>
     </row>
     <row r="36">
       <c r="A36" s="8" t="inlineStr">
@@ -11492,16 +11440,8 @@
           <t>vCenter Datastore Name</t>
         </is>
       </c>
-      <c r="B37" s="9" t="inlineStr">
-        <is>
-          <t>datastoreA</t>
-        </is>
-      </c>
-      <c r="C37" s="9" t="inlineStr">
-        <is>
-          <t>datastoreB</t>
-        </is>
-      </c>
+      <c r="B37" s="9" t="n"/>
+      <c r="C37" s="9" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="6" t="inlineStr">

</xml_diff>